<commit_message>
hsa: update the result of memory copy
</commit_message>
<xml_diff>
--- a/hsa/2_memory/result/data-all.xlsx
+++ b/hsa/2_memory/result/data-all.xlsx
@@ -492,58 +492,58 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.311167</v>
+        <v>0.30277</v>
       </c>
       <c r="D3">
-        <v>0.64046</v>
+        <v>0.622094</v>
       </c>
       <c r="E3">
-        <v>1.270747</v>
+        <v>1.273629</v>
       </c>
       <c r="F3">
-        <v>2.497591</v>
+        <v>2.487014</v>
       </c>
       <c r="G3">
-        <v>4.767245</v>
+        <v>4.664838</v>
       </c>
       <c r="H3">
-        <v>8.698916000000001</v>
+        <v>8.700206</v>
       </c>
       <c r="I3">
-        <v>14.968012</v>
+        <v>14.958417</v>
       </c>
       <c r="J3">
-        <v>23.411403</v>
+        <v>23.407006</v>
       </c>
       <c r="K3">
-        <v>31.337024</v>
+        <v>31.685974</v>
       </c>
       <c r="L3">
-        <v>40.513755</v>
+        <v>40.289131</v>
       </c>
       <c r="M3">
-        <v>45.089352</v>
+        <v>42.780729</v>
       </c>
       <c r="N3">
-        <v>42.572831</v>
+        <v>42.652847</v>
       </c>
       <c r="O3">
-        <v>44.788181</v>
+        <v>44.723804</v>
       </c>
       <c r="P3">
-        <v>48.490188</v>
+        <v>48.396205</v>
       </c>
       <c r="Q3">
-        <v>1030.905633</v>
+        <v>45.072236</v>
       </c>
       <c r="R3">
-        <v>1925.469332</v>
+        <v>45.223815</v>
       </c>
       <c r="S3">
-        <v>3459.910884</v>
+        <v>45.246745</v>
       </c>
       <c r="T3">
-        <v>7947.814743</v>
+        <v>45.144975</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -728,58 +728,58 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0.066068</v>
+        <v>0.065431</v>
       </c>
       <c r="D8">
-        <v>0.132792</v>
+        <v>0.132435</v>
       </c>
       <c r="E8">
-        <v>0.267959</v>
+        <v>0.266465</v>
       </c>
       <c r="F8">
-        <v>0.524851</v>
+        <v>0.516958</v>
       </c>
       <c r="G8">
-        <v>1.013797</v>
+        <v>0.995807</v>
       </c>
       <c r="H8">
-        <v>1.883735</v>
+        <v>1.858626</v>
       </c>
       <c r="I8">
-        <v>3.316726</v>
+        <v>3.273398</v>
       </c>
       <c r="J8">
-        <v>4.7526</v>
+        <v>4.763143</v>
       </c>
       <c r="K8">
-        <v>6.282248</v>
+        <v>6.20474</v>
       </c>
       <c r="L8">
-        <v>8.835601</v>
+        <v>8.658974000000001</v>
       </c>
       <c r="M8">
-        <v>10.730177</v>
+        <v>10.332109</v>
       </c>
       <c r="N8">
-        <v>11.727575</v>
+        <v>11.863943</v>
       </c>
       <c r="O8">
-        <v>12.86129</v>
+        <v>12.335983</v>
       </c>
       <c r="P8">
-        <v>13.243375</v>
+        <v>13.085151</v>
       </c>
       <c r="Q8">
-        <v>299.272494</v>
+        <v>13.359447</v>
       </c>
       <c r="R8">
-        <v>511.469301</v>
+        <v>13.33552</v>
       </c>
       <c r="S8">
-        <v>524.80717</v>
+        <v>13.351706</v>
       </c>
       <c r="T8">
-        <v>622.560082</v>
+        <v>13.457736</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -964,58 +964,58 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>0.06611</v>
+        <v>0.06561400000000001</v>
       </c>
       <c r="D13">
-        <v>0.134624</v>
+        <v>0.132676</v>
       </c>
       <c r="E13">
-        <v>0.269885</v>
+        <v>0.263979</v>
       </c>
       <c r="F13">
-        <v>0.5295570000000001</v>
+        <v>0.521127</v>
       </c>
       <c r="G13">
-        <v>1.02054</v>
+        <v>1.005211</v>
       </c>
       <c r="H13">
-        <v>1.879447</v>
+        <v>1.871335</v>
       </c>
       <c r="I13">
-        <v>3.333437</v>
+        <v>3.290276</v>
       </c>
       <c r="J13">
-        <v>4.819288</v>
+        <v>4.756716</v>
       </c>
       <c r="K13">
-        <v>6.220057</v>
+        <v>6.307795</v>
       </c>
       <c r="L13">
-        <v>8.667695999999999</v>
+        <v>8.823107</v>
       </c>
       <c r="M13">
-        <v>11.105345</v>
+        <v>10.582898</v>
       </c>
       <c r="N13">
-        <v>11.908145</v>
+        <v>11.807048</v>
       </c>
       <c r="O13">
-        <v>12.753252</v>
+        <v>12.809033</v>
       </c>
       <c r="P13">
-        <v>13.319682</v>
+        <v>13.124515</v>
       </c>
       <c r="Q13">
-        <v>240.184477</v>
+        <v>13.649282</v>
       </c>
       <c r="R13">
-        <v>304.053843</v>
+        <v>13.692114</v>
       </c>
       <c r="S13">
-        <v>362.87885</v>
+        <v>13.660944</v>
       </c>
       <c r="T13">
-        <v>505.719358</v>
+        <v>13.316356</v>
       </c>
     </row>
     <row r="14" spans="1:20">

</xml_diff>